<commit_message>
change Analize Excel file to month/month
</commit_message>
<xml_diff>
--- a/data/Analyze_file.xlsx
+++ b/data/Analyze_file.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تفریح" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="حمل و نقل" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="اینترنت" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="پوشاک" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="کمکی" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="اموزشی" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="دانشگاه" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="پس انداز" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="سلامت" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="result" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="تفریح" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="حمل و نقل" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="اینترنت" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="پوشاک" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="کمکی" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="اموزشی" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="دانشگاه" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="پس انداز" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="سلامت" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="result" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -62,6 +62,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -528,7 +596,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -543,7 +611,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -558,7 +626,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
@@ -620,7 +688,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -635,7 +703,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -650,7 +718,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -712,7 +780,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -727,7 +795,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -742,7 +810,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -804,7 +872,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -819,7 +887,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -834,7 +902,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
@@ -896,7 +964,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -911,7 +979,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -926,7 +994,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
@@ -988,7 +1056,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -1003,7 +1071,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -1018,7 +1086,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
@@ -1080,7 +1148,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -1095,7 +1163,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -1110,7 +1178,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
@@ -1172,7 +1240,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -1187,7 +1255,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -1202,7 +1270,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C72" t="inlineStr">
         <is>
@@ -1264,7 +1332,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -1279,7 +1347,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -1294,7 +1362,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C80" t="inlineStr">
         <is>
@@ -1356,7 +1424,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -1371,7 +1439,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -1386,7 +1454,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
@@ -1448,7 +1516,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>200000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -1463,7 +1531,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -1478,7 +1546,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>160000</v>
+        <v>0</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -1873,7 +1941,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1888,7 +1956,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -1903,7 +1971,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
@@ -1965,7 +2033,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -1980,7 +2048,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -1995,7 +2063,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -2057,7 +2125,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -2072,7 +2140,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -2087,7 +2155,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
@@ -2149,7 +2217,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -2164,7 +2232,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -2179,7 +2247,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -2241,7 +2309,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -2256,7 +2324,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -2271,7 +2339,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
@@ -2333,7 +2401,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -2348,7 +2416,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -2363,7 +2431,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
@@ -2425,7 +2493,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -2440,7 +2508,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -2455,7 +2523,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
@@ -2517,7 +2585,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -2532,7 +2600,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -2547,7 +2615,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
@@ -2609,7 +2677,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -2624,7 +2692,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -2639,7 +2707,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
@@ -2701,7 +2769,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -2716,7 +2784,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -2731,7 +2799,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C87" t="inlineStr">
         <is>
@@ -2793,7 +2861,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -2808,7 +2876,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -2823,7 +2891,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -2996,7 +3064,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -3026,7 +3094,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -3088,7 +3156,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -3118,7 +3186,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -3180,7 +3248,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -3210,7 +3278,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -3272,7 +3340,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -3302,7 +3370,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -3364,7 +3432,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -3394,7 +3462,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -3456,7 +3524,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -3486,7 +3554,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -3548,7 +3616,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -3578,7 +3646,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -3640,7 +3708,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -3670,7 +3738,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -3732,7 +3800,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3762,7 +3830,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -3824,7 +3892,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -3854,7 +3922,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -3916,7 +3984,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -3946,7 +4014,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -4119,7 +4187,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -4149,7 +4217,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -4211,7 +4279,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -4241,7 +4309,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -4303,7 +4371,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -4333,7 +4401,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -4395,7 +4463,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -4425,7 +4493,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -4487,7 +4555,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -4517,7 +4585,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -4579,7 +4647,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -4609,7 +4677,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -4671,7 +4739,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -4701,7 +4769,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -4763,7 +4831,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -4793,7 +4861,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -4855,7 +4923,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -4885,7 +4953,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -4947,7 +5015,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -4977,7 +5045,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -5039,7 +5107,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -5069,7 +5137,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -5242,7 +5310,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -5272,7 +5340,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -5334,7 +5402,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -5364,7 +5432,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -5426,7 +5494,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -5456,7 +5524,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -5518,7 +5586,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -5548,7 +5616,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -5610,7 +5678,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -5640,7 +5708,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -5702,7 +5770,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -5732,7 +5800,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -5794,7 +5862,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -5824,7 +5892,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -5886,7 +5954,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -5916,7 +5984,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -5978,7 +6046,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -6008,7 +6076,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -6070,7 +6138,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -6100,7 +6168,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -6162,7 +6230,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -6192,7 +6260,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>40000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -6365,7 +6433,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -6395,7 +6463,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -6457,7 +6525,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -6487,7 +6555,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -6549,7 +6617,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -6579,7 +6647,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -6641,7 +6709,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -6671,7 +6739,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -6733,7 +6801,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -6763,7 +6831,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -6825,7 +6893,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -6855,7 +6923,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -6917,7 +6985,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -6947,7 +7015,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -7009,7 +7077,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -7039,7 +7107,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -7101,7 +7169,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -7131,7 +7199,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -7193,7 +7261,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -7223,7 +7291,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -7285,7 +7353,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -7315,7 +7383,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>50000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -7411,7 +7479,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -7426,7 +7494,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1400000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -7488,7 +7556,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -7503,7 +7571,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -7580,7 +7648,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -7595,7 +7663,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -7672,7 +7740,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -7687,7 +7755,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -7764,7 +7832,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -7779,7 +7847,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -7856,7 +7924,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -7871,7 +7939,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -7948,7 +8016,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -7963,7 +8031,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -8040,7 +8108,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -8055,7 +8123,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -8132,7 +8200,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -8147,7 +8215,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -8224,7 +8292,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -8239,7 +8307,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -8316,7 +8384,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -8331,7 +8399,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -8423,7 +8491,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>1400000</v>
+        <v>0</v>
       </c>
       <c r="C93" t="inlineStr">
         <is>
@@ -8453,7 +8521,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0</v>
+        <v>-1400000</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
@@ -8549,7 +8617,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -8564,7 +8632,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>600000</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -8626,7 +8694,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -8641,7 +8709,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -8718,7 +8786,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -8733,7 +8801,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -8810,7 +8878,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -8825,7 +8893,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -8902,7 +8970,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -8917,7 +8985,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C37" t="inlineStr">
         <is>
@@ -8994,7 +9062,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -9009,7 +9077,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
@@ -9086,7 +9154,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -9101,7 +9169,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
@@ -9178,7 +9246,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -9193,7 +9261,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
@@ -9270,7 +9338,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -9285,7 +9353,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
@@ -9362,7 +9430,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -9377,7 +9445,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
@@ -9454,7 +9522,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -9469,7 +9537,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
@@ -9576,7 +9644,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
@@ -9606,7 +9674,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>0</v>
+        <v>-600000</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
@@ -9779,7 +9847,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -9809,7 +9877,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -9871,7 +9939,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
@@ -9901,7 +9969,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
@@ -9963,7 +10031,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
@@ -9993,7 +10061,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
@@ -10055,7 +10123,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
@@ -10085,7 +10153,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -10147,7 +10215,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -10177,7 +10245,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
@@ -10239,7 +10307,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
@@ -10269,7 +10337,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
@@ -10331,7 +10399,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
@@ -10361,7 +10429,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
@@ -10423,7 +10491,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
@@ -10453,7 +10521,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
@@ -10515,7 +10583,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -10545,7 +10613,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
@@ -10607,7 +10675,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
@@ -10637,7 +10705,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
@@ -10699,7 +10767,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
@@ -10729,7 +10797,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>30000</v>
+        <v>0</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>

</xml_diff>